<commit_message>
add error deal for fd jcfx
</commit_message>
<xml_diff>
--- a/profile/新抖数据接口更新.xlsx
+++ b/profile/新抖数据接口更新.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xubinbin/Desktop/xd_crawler/profile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7AA7C4-955B-8148-BA48-9C0242E9035A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCE87B5-0E52-C047-86B7-C890931C5D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,12 +183,6 @@
     <t>livestraming_time</t>
   </si>
   <si>
-    <t>taffic_time</t>
-  </si>
-  <si>
-    <t>zxrs</t>
-  </si>
-  <si>
     <t>ljgk</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>dms</t>
   </si>
   <si>
-    <t>fst</t>
-  </si>
-  <si>
     <t>zzgm</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t>spsj_sales</t>
   </si>
   <si>
-    <t>jjsp_product</t>
-  </si>
-  <si>
     <t>jjsp_price</t>
   </si>
   <si>
@@ -264,21 +252,6 @@
     <t>图示编号</t>
   </si>
   <si>
-    <t>url_works</t>
-  </si>
-  <si>
-    <t>time_release</t>
-  </si>
-  <si>
-    <t>zdx</t>
-  </si>
-  <si>
-    <t>zbdz</t>
-  </si>
-  <si>
-    <t>ygyl</t>
-  </si>
-  <si>
     <t>总点赞</t>
   </si>
   <si>
@@ -298,12 +271,6 @@
   </si>
   <si>
     <t>cytj</t>
-  </si>
-  <si>
-    <t>cyrs</t>
-  </si>
-  <si>
-    <t>zjrs</t>
   </si>
   <si>
     <t>填充示例</t>
@@ -365,13 +332,57 @@
   <si>
     <t>https://xd.newrank.cn/broadcast/liveDetails/7050770023975652103#domId=trafficAnalysis</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cyrs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>zjrs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>url_works</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>time_release</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>zdx</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>zbdz</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygyl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>taffic_time</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>zxrs</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>fst</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jjsp_product</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +420,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -470,7 +489,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,6 +592,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -628,7 +653,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7620" y="7620"/>
-          <a:ext cx="9502140" cy="5052060"/>
+          <a:ext cx="10490637" cy="4907526"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3651,7 +3676,7 @@
   <dimension ref="A2:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="204" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3661,7 +3686,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -3735,7 +3760,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="A13" s="33" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
@@ -3767,7 +3792,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="A17" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
@@ -3986,7 +4011,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="30" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4005,8 +4030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A28:Q42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView zoomScale="186" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4124,43 +4149,43 @@
       <c r="G34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="I34" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="L34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="M34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="N34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="P34" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q34" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="2" customFormat="1">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
@@ -4215,49 +4240,49 @@
         <v>45</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="H38" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="I38" t="s">
         <v>67</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H38" t="s">
-        <v>70</v>
-      </c>
-      <c r="I38" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
       <c r="H39" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -4265,7 +4290,7 @@
     </row>
     <row r="42" spans="1:17">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4278,6 +4303,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4286,8 +4312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A25:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView zoomScale="192" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4300,7 +4326,7 @@
   <sheetData>
     <row r="25" spans="1:13">
       <c r="A25" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -4326,7 +4352,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
@@ -4387,31 +4413,31 @@
       <c r="G28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" t="s">
-        <v>81</v>
-      </c>
-      <c r="K28" t="s">
-        <v>82</v>
-      </c>
-      <c r="L28" t="s">
-        <v>83</v>
+      <c r="H28" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="L28" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="M28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -4421,16 +4447,16 @@
       <c r="H29" s="13"/>
       <c r="I29" s="16"/>
       <c r="J29" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="K29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="L29" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4447,8 +4473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A37:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4458,7 +4484,7 @@
   <sheetData>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -4536,30 +4562,30 @@
         <v>51</v>
       </c>
       <c r="H40" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I40" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J40" t="s">
-        <v>90</v>
-      </c>
-      <c r="K40" t="s">
-        <v>91</v>
-      </c>
-      <c r="L40" t="s">
-        <v>92</v>
+        <v>81</v>
+      </c>
+      <c r="K40" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="L40" s="34" t="s">
+        <v>103</v>
       </c>
       <c r="M40" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C41" s="28"/>
       <c r="D41" s="28"/>
@@ -4567,22 +4593,22 @@
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
       <c r="H41" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I41" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="J41" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K41" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="L41" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4600,7 +4626,7 @@
   <dimension ref="A19:M24"/>
   <sheetViews>
     <sheetView zoomScale="180" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24:L24"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4701,30 +4727,30 @@
         <v>51</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
@@ -4733,15 +4759,15 @@
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="K23" s="29"/>
       <c r="L23" s="29"/>
       <c r="M23" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -4753,10 +4779,10 @@
       <c r="G24" s="5"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
@@ -4864,21 +4890,21 @@
         <v>51</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
@@ -4886,21 +4912,21 @@
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="29" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
     </row>
     <row r="26" spans="1:10">
       <c r="H26" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="6" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>